<commit_message>
adding additional information to STORMS
</commit_message>
<xml_diff>
--- a/STORMS_guidelines.xlsx
+++ b/STORMS_guidelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfrance/bioinformatics_analysis/small_projects/2year/Two_year/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C400DCD7-F539-B54B-987F-5B8B67A41A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687043EE-245C-134A-A162-A90DBFF66426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="612">
   <si>
     <t>STORMS</t>
   </si>
@@ -2175,6 +2175,9 @@
   </si>
   <si>
     <t>Secondary analysis of samples described in a prior study</t>
+  </si>
+  <si>
+    <t>Shotgun metagenomics, HiSeq 2500</t>
   </si>
 </sst>
 </file>
@@ -2984,8 +2987,8 @@
   <dimension ref="A1:Y1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3663,7 +3666,9 @@
       <c r="F33" s="49" t="s">
         <v>608</v>
       </c>
-      <c r="G33" s="104"/>
+      <c r="G33" s="104" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="34" spans="1:7" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="60">

</xml_diff>